<commit_message>
Updated 02.12.2021, ~1pm CST
</commit_message>
<xml_diff>
--- a/Categories Assignment.xlsx
+++ b/Categories Assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\311 Data\Math 5545 Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64e1b9c56e7ec9ea/Documents/UMKC/MATH 490/GP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C6644E-C0D9-448E-99B5-FAF9BF2CDF6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{80C6644E-C0D9-448E-99B5-FAF9BF2CDF6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F3EA0DB6-9782-4C17-A01C-8C598A2B646E}"/>
   <bookViews>
-    <workbookView xWindow="12030" yWindow="3120" windowWidth="14895" windowHeight="11385" xr2:uid="{7C30F52E-DFEE-471B-868A-F17E658BCBA7}"/>
+    <workbookView xWindow="-28920" yWindow="-135" windowWidth="29040" windowHeight="15840" xr2:uid="{7C30F52E-DFEE-471B-868A-F17E658BCBA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,80 +549,224 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>876</v>
+      </c>
+      <c r="C2">
+        <v>3430</v>
+      </c>
+      <c r="D2">
+        <v>672</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>125</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>299</v>
+      </c>
+      <c r="D6">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B7">
+        <v>229</v>
+      </c>
+      <c r="C7">
+        <v>1634</v>
+      </c>
+      <c r="D7">
+        <v>801</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B8">
+        <v>288</v>
+      </c>
+      <c r="C8">
+        <v>1184</v>
+      </c>
+      <c r="D8">
+        <v>246</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B9">
+        <v>61</v>
+      </c>
+      <c r="C9">
+        <v>327</v>
+      </c>
+      <c r="D9">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B10">
+        <v>958</v>
+      </c>
+      <c r="C10">
+        <v>5487</v>
+      </c>
+      <c r="D10">
+        <v>815</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B11">
+        <v>231</v>
+      </c>
+      <c r="C11">
+        <v>1060</v>
+      </c>
+      <c r="D11">
+        <v>141</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <v>160</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B13">
+        <v>47</v>
+      </c>
+      <c r="C13">
+        <v>456</v>
+      </c>
+      <c r="D13">
+        <v>272</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B14">
+        <v>150</v>
+      </c>
+      <c r="C14">
+        <v>907</v>
+      </c>
+      <c r="D14">
+        <v>374</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B15">
+        <v>253</v>
+      </c>
+      <c r="C15">
+        <v>1509</v>
+      </c>
+      <c r="D15">
+        <v>471</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>755</v>
+      </c>
+      <c r="C16">
+        <v>6428</v>
+      </c>
+      <c r="D16">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="B17">
+        <v>2211</v>
+      </c>
+      <c r="C17">
+        <v>11565</v>
+      </c>
+      <c r="D17">
+        <v>4400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>